<commit_message>
Thesis revision on 8/15.
</commit_message>
<xml_diff>
--- a/Thesis-codes/Exp-12/comparison.xlsx
+++ b/Thesis-codes/Exp-12/comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MPhil-thesis-github-library\MPhil-thesis\Thesis-codes\Exp-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CC77C7-C2CB-4AE3-933D-CA9D1EB78A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A250DC-ABEB-43A1-B637-25EB72ABCA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4183" yWindow="2289" windowWidth="19834" windowHeight="10765" xr2:uid="{E6A9F217-9E30-4D26-B398-62BD35DE3615}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="27960" windowHeight="13149" xr2:uid="{E6A9F217-9E30-4D26-B398-62BD35DE3615}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
     <t>lstm4</t>
   </si>
   <si>
-    <t>e</t>
+    <t>lstm3</t>
   </si>
 </sst>
 </file>
@@ -87,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -112,12 +112,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,7 +139,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -142,12 +148,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE432EB-879D-41FE-9802-14A816143173}">
-  <dimension ref="I7:P16"/>
+  <dimension ref="I7:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -475,248 +483,372 @@
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="9:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J7" s="2">
         <v>5</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
         <v>2</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2"/>
+      <c r="N7" s="2">
         <v>1</v>
       </c>
-      <c r="M7" s="2">
+      <c r="O7" s="2"/>
+      <c r="P7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="9:16" x14ac:dyDescent="0.4">
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J8" s="2">
         <v>5</v>
       </c>
-      <c r="K8" s="2">
-        <v>4</v>
-      </c>
+      <c r="K8" s="2"/>
       <c r="L8" s="2">
         <v>4</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="2"/>
+      <c r="N8" s="2">
+        <v>4</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="9:16" x14ac:dyDescent="0.4">
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="2"/>
+      <c r="P9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N9" t="s">
+      <c r="Q9" s="3"/>
+      <c r="R9" t="s">
         <v>14</v>
       </c>
-      <c r="O9" t="s">
+      <c r="T9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="9:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J10" s="4">
         <v>1.38E-2</v>
       </c>
-      <c r="K10" s="4">
-        <v>1.38E-2</v>
+      <c r="K10" s="1">
+        <f>($T10-J10)/$T10</f>
+        <v>1.4285714285714323E-2</v>
       </c>
       <c r="L10" s="4">
         <v>1.38E-2</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="1">
+        <f>($T10-L10)/$T10</f>
+        <v>1.4285714285714323E-2</v>
+      </c>
+      <c r="N10" s="4">
+        <v>1.38E-2</v>
+      </c>
+      <c r="O10" s="1">
+        <f>($T10-N10)/$T10</f>
+        <v>1.4285714285714323E-2</v>
+      </c>
+      <c r="P10" s="5">
         <v>1.3899999999999999E-2</v>
       </c>
-      <c r="N10">
+      <c r="Q10" s="1">
+        <f>($T10-P10)/$T10</f>
+        <v>7.1428571428572233E-3</v>
+      </c>
+      <c r="R10" s="6">
         <v>1.35E-2</v>
       </c>
-      <c r="O10">
+      <c r="S10" s="1">
+        <f>($R10-P10)/$R10</f>
+        <v>-2.9629629629629579E-2</v>
+      </c>
+      <c r="T10" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="P10" s="1">
-        <f>(O10-M10)/O10</f>
-        <v>7.1428571428572233E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="9:16" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J11" s="4">
         <v>1.47E-2</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="1">
+        <f>($T11-J11)/$T11</f>
+        <v>5.1612903225806472E-2</v>
+      </c>
+      <c r="L11" s="4">
         <v>1.54E-2</v>
       </c>
-      <c r="L11" s="4">
+      <c r="M11" s="1">
+        <f>($T11-L11)/$T11</f>
+        <v>6.4516129032257674E-3</v>
+      </c>
+      <c r="N11" s="4">
         <v>1.49E-2</v>
       </c>
-      <c r="M11" s="5">
+      <c r="O11" s="1">
+        <f>($T11-N11)/$T11</f>
+        <v>3.8709677419354827E-2</v>
+      </c>
+      <c r="P11" s="5">
         <v>1.4E-2</v>
       </c>
-      <c r="N11">
+      <c r="Q11" s="1">
+        <f>($T11-P11)/$T11</f>
+        <v>9.6774193548387066E-2</v>
+      </c>
+      <c r="R11" s="6">
         <v>1.44E-2</v>
       </c>
-      <c r="O11">
+      <c r="S11" s="1">
+        <f t="shared" ref="S11:S16" si="0">($R11-P11)/$R11</f>
+        <v>2.7777777777777731E-2</v>
+      </c>
+      <c r="T11" s="6">
         <v>1.55E-2</v>
       </c>
-      <c r="P11" s="1">
-        <f t="shared" ref="P11:P16" si="0">(O11-M11)/O11</f>
-        <v>9.6774193548387066E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="9:16" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J12" s="4">
         <v>1.41E-2</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="1">
+        <f>($T12-J12)/$T12</f>
+        <v>-3.6764705882352977E-2</v>
+      </c>
+      <c r="L12" s="4">
         <v>1.38E-2</v>
       </c>
-      <c r="L12" s="4">
+      <c r="M12" s="1">
+        <f>($T12-L12)/$T12</f>
+        <v>-1.4705882352941216E-2</v>
+      </c>
+      <c r="N12" s="4">
         <v>1.41E-2</v>
       </c>
-      <c r="M12" s="5">
+      <c r="O12" s="1">
+        <f>($T12-N12)/$T12</f>
+        <v>-3.6764705882352977E-2</v>
+      </c>
+      <c r="P12" s="5">
         <v>1.34E-2</v>
       </c>
-      <c r="N12">
+      <c r="Q12" s="1">
+        <f>($T12-P12)/$T12</f>
+        <v>1.4705882352941088E-2</v>
+      </c>
+      <c r="R12" s="6">
         <v>1.43E-2</v>
       </c>
-      <c r="O12">
+      <c r="S12" s="1">
+        <f t="shared" si="0"/>
+        <v>6.2937062937062915E-2</v>
+      </c>
+      <c r="T12" s="6">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="P12" s="1">
-        <f t="shared" si="0"/>
-        <v>1.4705882352941088E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="9:16" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J13" s="4">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="1">
+        <f>($T13-J13)/$T13</f>
+        <v>-1.5503875968992289E-2</v>
+      </c>
+      <c r="L13" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="L13" s="4">
+      <c r="M13" s="1">
+        <f>($T13-L13)/$T13</f>
+        <v>-7.7519379844960771E-3</v>
+      </c>
+      <c r="N13" s="4">
         <v>1.37E-2</v>
       </c>
-      <c r="M13" s="5">
+      <c r="O13" s="1">
+        <f>($T13-N13)/$T13</f>
+        <v>-6.2015503875969019E-2</v>
+      </c>
+      <c r="P13" s="5">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="N13">
+      <c r="Q13" s="1">
+        <f>($T13-P13)/$T13</f>
+        <v>-7.7519379844960771E-3</v>
+      </c>
+      <c r="R13" s="7">
         <v>1.2E-2</v>
       </c>
-      <c r="O13">
+      <c r="S13" s="1">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333333259E-2</v>
+      </c>
+      <c r="T13" s="6">
         <v>1.29E-2</v>
       </c>
-      <c r="P13" s="1">
-        <f t="shared" si="0"/>
-        <v>-7.7519379844960771E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="9:16" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J14" s="4">
         <v>1.3899999999999999E-2</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="1">
+        <f>($T14-J14)/$T14</f>
+        <v>1.4184397163120605E-2</v>
+      </c>
+      <c r="L14" s="4">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="L14" s="4">
+      <c r="M14" s="1">
+        <f>($T14-L14)/$T14</f>
+        <v>3.5460992907801449E-2</v>
+      </c>
+      <c r="N14" s="4">
         <v>1.37E-2</v>
       </c>
-      <c r="M14" s="5">
+      <c r="O14" s="1">
+        <f>($T14-N14)/$T14</f>
+        <v>2.8368794326241085E-2</v>
+      </c>
+      <c r="P14" s="5">
         <v>1.29E-2</v>
       </c>
-      <c r="N14">
+      <c r="Q14" s="1">
+        <f>($T14-P14)/$T14</f>
+        <v>8.5106382978723388E-2</v>
+      </c>
+      <c r="R14" s="6">
         <v>1.32E-2</v>
       </c>
-      <c r="O14">
+      <c r="S14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2727272727272721E-2</v>
+      </c>
+      <c r="T14" s="6">
         <v>1.41E-2</v>
       </c>
-      <c r="P14" s="1">
-        <f t="shared" si="0"/>
-        <v>8.5106382978723388E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="9:16" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J15" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="1">
+        <f>($T15-J15)/$T15</f>
+        <v>7.3529411764705439E-3</v>
+      </c>
+      <c r="L15" s="4">
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="L15" s="4">
+      <c r="M15" s="1">
+        <f>($T15-L15)/$T15</f>
+        <v>-4.411764705882365E-2</v>
+      </c>
+      <c r="N15" s="4">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="M15" s="5">
+      <c r="O15" s="1">
+        <f>($T15-N15)/$T15</f>
+        <v>2.2058823529411759E-2</v>
+      </c>
+      <c r="P15" s="5">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="N15">
+      <c r="Q15" s="1">
+        <f>($T15-P15)/$T15</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="6">
         <v>1.34E-2</v>
       </c>
-      <c r="O15">
+      <c r="S15" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.4925373134328268E-2</v>
+      </c>
+      <c r="T15" s="6">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="P15" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="9:16" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="9:20" x14ac:dyDescent="0.4">
       <c r="I16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="J16" s="4">
         <v>1.35E-2</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="1">
+        <f>($T16-J16)/$T16</f>
+        <v>1.4598540145985439E-2</v>
+      </c>
+      <c r="L16" s="4">
         <v>1.3899999999999999E-2</v>
       </c>
-      <c r="L16" s="4">
+      <c r="M16" s="1">
+        <f>($T16-L16)/$T16</f>
+        <v>-1.4598540145985313E-2</v>
+      </c>
+      <c r="N16" s="4">
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="M16" s="5">
+      <c r="O16" s="1">
+        <f>($T16-N16)/$T16</f>
+        <v>-3.6496350364963535E-2</v>
+      </c>
+      <c r="P16" s="5">
         <v>1.26E-2</v>
       </c>
-      <c r="N16">
+      <c r="Q16" s="1">
+        <f>($T16-P16)/$T16</f>
+        <v>8.0291970802919721E-2</v>
+      </c>
+      <c r="R16" s="6">
         <v>1.35E-2</v>
       </c>
-      <c r="O16">
+      <c r="S16" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666652E-2</v>
+      </c>
+      <c r="T16" s="6">
         <v>1.37E-2</v>
-      </c>
-      <c r="P16" s="1">
-        <f t="shared" si="0"/>
-        <v>8.0291970802919721E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>